<commit_message>
add mail and fixes
</commit_message>
<xml_diff>
--- a/public/sheets/record.xlsx
+++ b/public/sheets/record.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Tên</t>
   </si>
@@ -35,31 +35,21 @@
     <t>Trần Thị Long Lanh Sương Sớm Mai</t>
   </si>
   <si>
-    <t>Ăn quà sai quy định 10/11/2023 (admin, 15); Đi trễ 12/11/2023 (admin, 20);</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>Không thuộc bài 10/11/2023 (admin, 5);</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị E</t>
-  </si>
-  <si>
-    <t>Đi trễ 10/11/2023 (admin, 3); Đi trễ 10/11/2023 (admin, 6);</t>
+    <t>Đi trễ 12/11/2023 (admin, 20)</t>
   </si>
   <si>
     <t>Nguyễn Lê Phi Long</t>
   </si>
   <si>
-    <t>Đi trễ 12/11/2023 (admin, 21);</t>
+    <t>Đi trễ 12/11/2023 (admin, 21)</t>
   </si>
   <si>
     <t>Phan Hoài Linh</t>
   </si>
   <si>
-    <t>Ăn quà sai quy định 10/11/2023 (admin, 4); Ăn quà sai quy định 10/11/2023 (admin, 16); Ăn quà sai quy định 12/11/2023 (admin, 17); Ăn quà sai quy định 12/11/2023 (admin, 18); Ăn quà sai quy định 12/11/2023 (admin, 19);</t>
+    <t>Ăn quà sai quy định 12/11/2023 (admin, 17)
+Ăn quà sai quy định 12/11/2023 (admin, 18)
+Ăn quà sai quy định 12/11/2023 (admin, 19)</t>
   </si>
 </sst>
 </file>
@@ -402,10 +392,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,7 +404,7 @@
     <col min="2" max="2" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="258.223" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="50.559" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -435,88 +425,54 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>12.09</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>12.01</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>12.05</v>
+      </c>
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>12.04</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="1">
+        <v>12.05</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>12.05</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>12.05</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>